<commit_message>
Initial addition of hierarchical clustering
</commit_message>
<xml_diff>
--- a/Nextera PCR for all 25 tissues and 5 in vitro samples.xlsx
+++ b/Nextera PCR for all 25 tissues and 5 in vitro samples.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="73">
   <si>
     <t>Index 1 (i7)</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>Amount(ng)</t>
+  </si>
+  <si>
+    <t>Cell type</t>
+  </si>
+  <si>
+    <t>293T</t>
+  </si>
+  <si>
+    <t>Mouse primary cortical neurons</t>
   </si>
 </sst>
 </file>
@@ -305,8 +314,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -462,7 +475,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -530,6 +543,8 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -597,6 +612,8 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1980,7 +1997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="7" customFormat="1">
+    <row r="33" spans="1:13" s="7" customFormat="1">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="3"/>
@@ -1994,7 +2011,7 @@
       <c r="K33"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="G34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2004,8 +2021,11 @@
       <c r="I34" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="6">
         <v>26</v>
       </c>
@@ -2043,8 +2063,11 @@
       <c r="L35" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="6">
         <v>27</v>
       </c>
@@ -2082,8 +2105,11 @@
       <c r="L36" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="6">
         <v>28</v>
       </c>
@@ -2121,8 +2147,11 @@
       <c r="L37" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="6">
         <v>29</v>
       </c>
@@ -2160,8 +2189,11 @@
       <c r="L38" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="6">
         <v>30</v>
       </c>
@@ -2199,8 +2231,11 @@
       <c r="L39" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="H40" s="6"/>
       <c r="K40">
         <f>SUM(K2:K39)</f>

</xml_diff>